<commit_message>
+ added more outputs
</commit_message>
<xml_diff>
--- a/outputs/_overview.xlsx
+++ b/outputs/_overview.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelda\Desktop\repositories\github\python-pysml-covid19\outputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbit/Desktop/repositories/github/python-pysml-covid19/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDDD7819-4061-43EC-9B94-433E2813B142}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A36835F-87B6-3D4E-9D49-2F913B653E95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15920" yWindow="460" windowWidth="19900" windowHeight="21940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="1" r:id="rId1"/>
+    <sheet name="Panel" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="87">
   <si>
     <t>id_data</t>
   </si>
@@ -126,6 +127,174 @@
   </si>
   <si>
     <t>ann-none-median-smote-std-skfold-21</t>
+  </si>
+  <si>
+    <t>gnb-none-median-smote-std-skfold-21</t>
+  </si>
+  <si>
+    <t>Biomarker</t>
+  </si>
+  <si>
+    <t>Panel</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>WBC</t>
+  </si>
+  <si>
+    <t>HGB</t>
+  </si>
+  <si>
+    <t>HCT</t>
+  </si>
+  <si>
+    <t>RDW</t>
+  </si>
+  <si>
+    <t>MCV</t>
+  </si>
+  <si>
+    <t>MCHC</t>
+  </si>
+  <si>
+    <t>RBC</t>
+  </si>
+  <si>
+    <t>PLT</t>
+  </si>
+  <si>
+    <t>UREA</t>
+  </si>
+  <si>
+    <t>MPV</t>
+  </si>
+  <si>
+    <t>EGFR</t>
+  </si>
+  <si>
+    <t>CRE</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>SODIUM</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>NRBCA</t>
+  </si>
+  <si>
+    <t>NEUT</t>
+  </si>
+  <si>
+    <t>BALSO</t>
+  </si>
+  <si>
+    <t>LY</t>
+  </si>
+  <si>
+    <t>EOS</t>
+  </si>
+  <si>
+    <t>MONO</t>
+  </si>
+  <si>
+    <t>CRP</t>
+  </si>
+  <si>
+    <t>ALB</t>
+  </si>
+  <si>
+    <t>ALP</t>
+  </si>
+  <si>
+    <t>ALT</t>
+  </si>
+  <si>
+    <t>BIL</t>
+  </si>
+  <si>
+    <t>PHOS</t>
+  </si>
+  <si>
+    <t>CALC</t>
+  </si>
+  <si>
+    <t>CALCOR</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>GLOB</t>
+  </si>
+  <si>
+    <t>RPT</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>FIB</t>
+  </si>
+  <si>
+    <t>PT</t>
+  </si>
+  <si>
+    <t>APTT</t>
+  </si>
+  <si>
+    <t>HCT HGB</t>
+  </si>
+  <si>
+    <t>PANEL_FBC</t>
+  </si>
+  <si>
+    <t>Full Blood Count</t>
+  </si>
+  <si>
+    <t>PANEL_U&amp;E</t>
+  </si>
+  <si>
+    <t>Urea and Electrolites</t>
+  </si>
+  <si>
+    <t>PANEL_LFT</t>
+  </si>
+  <si>
+    <t>Lifer function test</t>
+  </si>
+  <si>
+    <t>PANEL_BONE</t>
+  </si>
+  <si>
+    <t>CALCOR is relation between CALC and ALB - linear equation (BEST)</t>
+  </si>
+  <si>
+    <t>TP = total protein hardly used</t>
+  </si>
+  <si>
+    <t>PANEL_CLOTING</t>
+  </si>
+  <si>
+    <t>PANEL_LFT (?)</t>
+  </si>
+  <si>
+    <t>PANEL_CRP</t>
+  </si>
+  <si>
+    <t>blood samples</t>
+  </si>
+  <si>
+    <t>Different concatiner different quemicals in the container for differents profiles</t>
+  </si>
+  <si>
+    <t>NEUT _ LY _ EOS _ BASO = WBC (ROGUHLY)</t>
   </si>
 </sst>
 </file>
@@ -134,9 +303,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +317,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -197,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -219,17 +394,41 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="19">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
@@ -238,6 +437,32 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -265,14 +490,16 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -289,6 +516,38 @@
           <color indexed="64"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -415,7 +674,158 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1100" baseline="0"/>
-            <a:t> dataset has patient nhs numbers with confirmed (positive/negative) covid outcomes. These have been merged with all the pathology data provided by Bernard. As such, the resulting file one_line_values_pathology.csv has the daily profiles for the patients (taking into account any existing biomarker) with the covid detection outcome. Using the previous described dataset we have evaluated a number of models to estimate the likelihood of positive covid outcome.</a:t>
+            <a:t> dataset has patient nhs numbers with confirmed (positive/negative) covid outcomes. These have been merged with all the pathology data provided by Bernard and the microbiology data provided by Nisha. As such, the resulting file daily_profiles.csv has the daily profiles for the patients (taking into account any existing biomarker) with the covid detection and microbiology outcomes. Using the previous described dataset we have evaluated a number of models to estimate the likelihood of positive covid outcome.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t>Notes:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1" baseline="0"/>
+            <a:t>   - </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>The algorithms XGBoost and LightGBM have not been tried (issues installing them in windows).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>   - The number of procalcitonin (PCT) records is too low and limits the number of daily profiles for training/testing.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t>   - In order to select the best algorithm looking at the highest gmean (balanced sensitivity and specificity).</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>428624</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A357C18-DD03-B041-8DB3-D89675C115BE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="825499" y="247650"/>
+          <a:ext cx="13662025" cy="2686050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-GB" sz="1400" b="1"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1400" b="1"/>
+            <a:t>EXPERIMENT II</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="1"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:t>Title: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0"/>
+            <a:t>Inference</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="0" baseline="0"/>
+            <a:t> of micro outcome</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100" b="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" b="1"/>
+            <a:t>Description: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>The dataset</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> provided by K</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>eira</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> dataset has patient nhs numbers with confirmed (positive/negative) covid outcomes. These have been merged with all the pathology data provided by Bernard and the microbiology data provided by Nisha. As such, the resulting file daily_profiles.csv has the daily profiles for the patients (taking into account any existing biomarker) with the covid detection and microbiology outcomes. Using the previous described dataset we have evaluated a number of models to estimate the likelihood of positive covid outcome.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -460,7 +870,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB689510-BE34-4901-9A29-69F4E836B24D}" name="Table1" displayName="Table1" ref="B17:S39" headerRowDxfId="3" headerRowBorderDxfId="5" tableBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DB689510-BE34-4901-9A29-69F4E836B24D}" name="Table1" displayName="Table1" ref="B17:S39" headerRowDxfId="18" headerRowBorderDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="B17:S39" xr:uid="{330E4312-09AE-42ED-8D68-2DE6BF49C53F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -482,7 +892,7 @@
     <filterColumn colId="17" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="18">
-    <tableColumn id="1" xr3:uid="{526CF63F-E032-46AC-928C-05F7424290C6}" name="algorithm" totalsRowLabel="Total" dataDxfId="4" totalsRowDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{526CF63F-E032-46AC-928C-05F7424290C6}" name="algorithm" totalsRowLabel="Total" dataDxfId="15" totalsRowDxfId="14"/>
     <tableColumn id="2" xr3:uid="{6918553E-ABFD-4094-A931-662F5EB13479}" name="features"/>
     <tableColumn id="3" xr3:uid="{9C39B3F3-1E62-4947-8BC2-EACF892F89EA}" name="id_data"/>
     <tableColumn id="4" xr3:uid="{B5DA5FF0-4E62-4BCC-AFBE-CC05714D40A9}" name="id_estm"/>
@@ -498,10 +908,59 @@
     <tableColumn id="14" xr3:uid="{4F5BDFD4-8824-499B-9737-6D45A979D259}" name="tn"/>
     <tableColumn id="15" xr3:uid="{37C338CB-54C6-4756-9862-D72982CAC3D1}" name="fp"/>
     <tableColumn id="16" xr3:uid="{8079B4C5-DFF2-4A96-8EE2-5E0103B48776}" name="fn"/>
-    <tableColumn id="17" xr3:uid="{F711BCF3-CDD8-4F5B-AEAB-F35CB5703D84}" name="sp0" dataDxfId="1"/>
-    <tableColumn id="18" xr3:uid="{A3F0C832-6112-4943-B593-48B7556A814F}" name="sp1" totalsRowFunction="sum" dataDxfId="0"/>
+    <tableColumn id="17" xr3:uid="{F711BCF3-CDD8-4F5B-AEAB-F35CB5703D84}" name="sp0" dataDxfId="13"/>
+    <tableColumn id="18" xr3:uid="{A3F0C832-6112-4943-B593-48B7556A814F}" name="sp1" totalsRowFunction="sum" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{369E845B-5219-5440-B98E-A28DF5C4CAD5}" name="Table13" displayName="Table13" ref="B61:S84" headerRowDxfId="11" headerRowBorderDxfId="10" tableBorderDxfId="9">
+  <autoFilter ref="B61:S84" xr:uid="{F7B43E7C-060D-104D-900B-63255EBF8699}"/>
+  <tableColumns count="18">
+    <tableColumn id="1" xr3:uid="{45F18955-2B6D-1843-8D4C-E249277D1BBE}" name="algorithm" totalsRowLabel="Total" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{0210B46E-1FA3-154E-97F1-680F33293AC5}" name="features"/>
+    <tableColumn id="3" xr3:uid="{FBA93F40-739E-2C40-8C7D-05B218AC2052}" name="id_data"/>
+    <tableColumn id="4" xr3:uid="{9834D1DA-93F4-A04C-9A4B-CC51F4F1A36E}" name="id_estm"/>
+    <tableColumn id="5" xr3:uid="{866AA6E7-B72E-E947-BE24-B0F85063C938}" name="id_fold"/>
+    <tableColumn id="6" xr3:uid="{84FF0FD3-6B8A-494C-A95C-BD5E89E0CBB3}" name="roc"/>
+    <tableColumn id="7" xr3:uid="{2E20B044-FCE8-4246-9868-E89BF3E39935}" name="prauc"/>
+    <tableColumn id="8" xr3:uid="{28368E8C-2BC3-334C-8526-F9FFBD5F0A57}" name="sens"/>
+    <tableColumn id="9" xr3:uid="{7EB5DF6A-4DB4-FD4C-9E40-46E3DF155597}" name="spec"/>
+    <tableColumn id="10" xr3:uid="{0A2F34B3-CAF0-EA40-B7C9-EDFAFAE315C0}" name="gmean"/>
+    <tableColumn id="11" xr3:uid="{F5D30D2E-4CFC-4943-A765-D4895F7A5ABD}" name="matt"/>
+    <tableColumn id="12" xr3:uid="{B6B1A3A5-6207-DD4C-A59C-36EEA4E1077C}" name="score"/>
+    <tableColumn id="13" xr3:uid="{6DDE3D41-7F3B-804C-A211-F641E7DB535A}" name="tp"/>
+    <tableColumn id="14" xr3:uid="{41055082-5CD7-D843-8B81-02CE78ABEEE5}" name="tn"/>
+    <tableColumn id="15" xr3:uid="{9B2980EC-3F07-4846-B48C-3D919B65F5FD}" name="fp"/>
+    <tableColumn id="16" xr3:uid="{BD9D5B92-C5F2-3046-B869-C164CEB94FE2}" name="fn"/>
+    <tableColumn id="17" xr3:uid="{45324D6B-94D3-8F40-A843-172D9FCB3A6D}" name="sp0" dataDxfId="6"/>
+    <tableColumn id="18" xr3:uid="{CB7AEDA7-1E1D-8147-83B3-EE7C260E5064}" name="sp1" totalsRowFunction="sum" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium25" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{38CA2FA7-0B25-5941-8AB7-19341C32CC4A}" name="Table4" displayName="Table4" ref="B5:C45" totalsRowShown="0" headerRowDxfId="1" dataDxfId="4">
+  <autoFilter ref="B5:C45" xr:uid="{77863DC7-B82D-F04A-8D36-6611600F6EA2}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{CE34B3F7-541D-EA43-A2F2-BB6965C3C62B}" name="Biomarker" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{AB14862E-EF6D-2549-99FB-402043C9D82D}" name="Panel" dataDxfId="3"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5F507699-0374-2F40-B440-F4C598DA2982}" name="Table5" displayName="Table5" ref="E5:F30" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="E5:F30" xr:uid="{740808C0-8A66-FF49-B9D9-5033F495B580}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{81CBF0A6-9B52-504C-B1FB-7692C7927960}" name="Panel"/>
+    <tableColumn id="2" xr3:uid="{2FEB4CF3-19D8-1F46-97B7-7EBE9F173A75}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -768,33 +1227,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B16:V42"/>
+  <dimension ref="B16:S84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G69" sqref="G69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="7" max="7" width="5.83203125" customWidth="1"/>
     <col min="8" max="8" width="8" customWidth="1"/>
-    <col min="9" max="10" width="7.140625" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="7.28515625" customWidth="1"/>
-    <col min="13" max="13" width="7.85546875" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="17" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.5703125" customWidth="1"/>
-    <col min="19" max="19" width="8.7109375" customWidth="1"/>
+    <col min="9" max="10" width="7.1640625" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" customWidth="1"/>
+    <col min="13" max="13" width="7.83203125" customWidth="1"/>
+    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.5" customWidth="1"/>
+    <col min="19" max="19" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="2:19" s="3" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="2:19" s="3" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="8" t="s">
         <v>17</v>
       </c>
@@ -850,7 +1309,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
         <v>19</v>
       </c>
@@ -906,7 +1365,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>20</v>
       </c>
@@ -962,7 +1421,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>21</v>
       </c>
@@ -1018,7 +1477,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B21" s="7" t="s">
         <v>22</v>
       </c>
@@ -1074,7 +1533,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
         <v>23</v>
       </c>
@@ -1130,7 +1589,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
         <v>24</v>
       </c>
@@ -1186,7 +1645,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B24" s="7" t="s">
         <v>29</v>
       </c>
@@ -1242,7 +1701,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B25" s="7" t="s">
         <v>25</v>
       </c>
@@ -1298,7 +1757,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B26" s="7" t="s">
         <v>26</v>
       </c>
@@ -1352,7 +1811,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B27" s="7" t="s">
         <v>27</v>
       </c>
@@ -1406,7 +1865,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B28" s="7" t="s">
         <v>30</v>
       </c>
@@ -1459,7 +1918,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B29" s="7" t="s">
         <v>28</v>
       </c>
@@ -1513,7 +1972,7 @@
         <v>1139</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B30" s="7"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1533,7 +1992,7 @@
       <c r="R30" s="15"/>
       <c r="S30" s="15"/>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B31" s="7"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1553,7 +2012,7 @@
       <c r="R31" s="15"/>
       <c r="S31" s="15"/>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B32" s="7"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -1573,7 +2032,7 @@
       <c r="R32" s="15"/>
       <c r="S32" s="15"/>
     </row>
-    <row r="33" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B33" s="7"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -1593,7 +2052,7 @@
       <c r="R33" s="15"/>
       <c r="S33" s="15"/>
     </row>
-    <row r="34" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B34" s="7"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
@@ -1613,7 +2072,7 @@
       <c r="R34" s="15"/>
       <c r="S34" s="15"/>
     </row>
-    <row r="35" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B35" s="7"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
@@ -1633,7 +2092,7 @@
       <c r="R35" s="15"/>
       <c r="S35" s="15"/>
     </row>
-    <row r="36" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B36" s="7"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -1653,7 +2112,7 @@
       <c r="R36" s="15"/>
       <c r="S36" s="15"/>
     </row>
-    <row r="37" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B37" s="7"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -1673,7 +2132,7 @@
       <c r="R37" s="15"/>
       <c r="S37" s="15"/>
     </row>
-    <row r="38" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B38" s="7"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -1693,7 +2152,7 @@
       <c r="R38" s="15"/>
       <c r="S38" s="15"/>
     </row>
-    <row r="39" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B39" s="7"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -1713,59 +2172,1327 @@
       <c r="R39" s="15"/>
       <c r="S39" s="15"/>
     </row>
-    <row r="42" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="H42" t="s">
+    <row r="61" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B61" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E61" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F61" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H61" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I61" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="J61" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="K61" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L61" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M61" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="N61" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="O61" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="P61" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q61" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="R61" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="S61" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B62" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" s="1">
+        <v>6</v>
+      </c>
+      <c r="D62" t="s">
         <v>16</v>
       </c>
-      <c r="I42">
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>4.5</v>
+      </c>
+      <c r="G62">
+        <v>0.63918609084952205</v>
+      </c>
+      <c r="H62">
+        <v>0.44337556557540803</v>
+      </c>
+      <c r="I62">
+        <v>0.23124042879019899</v>
+      </c>
+      <c r="J62">
+        <v>0.86494762288477001</v>
+      </c>
+      <c r="K62">
+        <v>0.44549228599986401</v>
+      </c>
+      <c r="L62">
+        <v>0.12272122319411501</v>
+      </c>
+      <c r="M62">
+        <v>0.64646251319957704</v>
+      </c>
+      <c r="N62">
+        <v>151</v>
+      </c>
+      <c r="O62">
+        <v>1073.4000000000001</v>
+      </c>
+      <c r="P62">
+        <v>167.6</v>
+      </c>
+      <c r="Q62">
+        <v>502</v>
+      </c>
+      <c r="R62">
+        <v>1241</v>
+      </c>
+      <c r="S62">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="63" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B63" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C63" s="2">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>16</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>4.5</v>
+      </c>
+      <c r="G63">
+        <v>0.64583333333333304</v>
+      </c>
+      <c r="H63">
+        <v>0.72722026015463703</v>
+      </c>
+      <c r="I63">
+        <v>0.439285714285714</v>
+      </c>
+      <c r="J63">
+        <v>0.74444444444444402</v>
+      </c>
+      <c r="K63">
+        <v>0.56947505723537795</v>
+      </c>
+      <c r="L63">
+        <v>0.18777829950567301</v>
+      </c>
+      <c r="M63">
+        <v>0.55869565217391304</v>
+      </c>
+      <c r="N63">
+        <v>12.3</v>
+      </c>
+      <c r="O63">
+        <v>13.4</v>
+      </c>
+      <c r="P63">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Q63">
+        <v>15.7</v>
+      </c>
+      <c r="R63">
+        <v>18</v>
+      </c>
+      <c r="S63">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="64" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B64" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C64" s="2">
+        <v>21</v>
+      </c>
+      <c r="D64" t="s">
+        <v>16</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>4.5</v>
+      </c>
+      <c r="G64">
+        <v>0.68341602878138397</v>
+      </c>
+      <c r="H64">
+        <v>0.47362434145029397</v>
+      </c>
+      <c r="I64">
+        <v>0.71320422535211203</v>
+      </c>
+      <c r="J64">
+        <v>0.55226086956521703</v>
+      </c>
+      <c r="K64">
+        <v>0.62711589944301405</v>
+      </c>
+      <c r="L64">
+        <v>0.250710229137381</v>
+      </c>
+      <c r="M64">
+        <v>0.60547147846332905</v>
+      </c>
+      <c r="N64">
+        <v>405.1</v>
+      </c>
+      <c r="O64">
+        <v>635.1</v>
+      </c>
+      <c r="P64">
+        <v>514.9</v>
+      </c>
+      <c r="Q64">
+        <v>162.9</v>
+      </c>
+      <c r="R64">
+        <v>1150</v>
+      </c>
+      <c r="S64">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="65" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B65" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C65" s="2">
+        <v>27</v>
+      </c>
+      <c r="D65" t="s">
+        <v>16</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>4.5</v>
+      </c>
+      <c r="G65">
+        <v>0.69474563686466595</v>
+      </c>
+      <c r="H65">
+        <v>0.48065742088068403</v>
+      </c>
+      <c r="I65">
+        <v>0.75246478873239397</v>
+      </c>
+      <c r="J65">
+        <v>0.54269565217391302</v>
+      </c>
+      <c r="K65">
+        <v>0.637852661995015</v>
+      </c>
+      <c r="L65">
+        <v>0.28021042750214398</v>
+      </c>
+      <c r="M65">
+        <v>0.612048894062863</v>
+      </c>
+      <c r="N65">
+        <v>427.4</v>
+      </c>
+      <c r="O65">
+        <v>624.1</v>
+      </c>
+      <c r="P65">
+        <v>525.9</v>
+      </c>
+      <c r="Q65">
+        <v>140.6</v>
+      </c>
+      <c r="R65">
+        <v>1150</v>
+      </c>
+      <c r="S65">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="66" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B66" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C66" s="2">
+        <v>6</v>
+      </c>
+      <c r="D66" s="2"/>
+      <c r="E66" s="2"/>
+      <c r="F66" s="2"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="12"/>
+      <c r="O66" s="12"/>
+      <c r="P66" s="12"/>
+      <c r="Q66" s="12"/>
+      <c r="R66" s="15"/>
+      <c r="S66" s="15"/>
+    </row>
+    <row r="67" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B67" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C67" s="2">
+        <v>6</v>
+      </c>
+      <c r="D67" t="s">
+        <v>16</v>
+      </c>
+      <c r="E67">
+        <v>4</v>
+      </c>
+      <c r="F67">
+        <v>4.5</v>
+      </c>
+      <c r="G67">
+        <v>0.76437615764592304</v>
+      </c>
+      <c r="H67">
+        <v>0.62242252289127897</v>
+      </c>
+      <c r="I67">
+        <v>0.68606431852986205</v>
+      </c>
+      <c r="J67">
+        <v>0.72167606768734804</v>
+      </c>
+      <c r="K67">
+        <v>0.70358126279340305</v>
+      </c>
+      <c r="L67">
+        <v>0.39286612090725798</v>
+      </c>
+      <c r="M67">
+        <v>0.70939809926082298</v>
+      </c>
+      <c r="N67">
+        <v>448</v>
+      </c>
+      <c r="O67">
+        <v>895.6</v>
+      </c>
+      <c r="P67">
+        <v>345.4</v>
+      </c>
+      <c r="Q67">
+        <v>205</v>
+      </c>
+      <c r="R67">
+        <v>1241</v>
+      </c>
+      <c r="S67">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="68" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B68" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C68" s="2">
+        <v>7</v>
+      </c>
+      <c r="D68" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68">
+        <v>3</v>
+      </c>
+      <c r="F68">
+        <v>4.5</v>
+      </c>
+      <c r="G68">
+        <v>0.700992063492063</v>
+      </c>
+      <c r="H68">
+        <v>0.789192598429032</v>
+      </c>
+      <c r="I68">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="J68">
+        <v>0.75555555555555498</v>
+      </c>
+      <c r="K68">
+        <v>0.65755157423739796</v>
+      </c>
+      <c r="L68">
+        <v>0.325889719343888</v>
+      </c>
+      <c r="M68">
+        <v>0.64565217391304297</v>
+      </c>
+      <c r="N68">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="O68">
+        <v>13.6</v>
+      </c>
+      <c r="P68">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Q68">
+        <v>11.9</v>
+      </c>
+      <c r="R68">
+        <v>18</v>
+      </c>
+      <c r="S68">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="69" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B69" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C69" s="2">
+        <v>21</v>
+      </c>
+      <c r="D69" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69">
+        <v>3</v>
+      </c>
+      <c r="F69">
+        <v>4.5</v>
+      </c>
+      <c r="G69">
+        <v>0.91349946417636196</v>
+      </c>
+      <c r="H69">
+        <v>0.85324351523446695</v>
+      </c>
+      <c r="I69">
+        <v>0.80052816901408397</v>
+      </c>
+      <c r="J69">
+        <v>0.89017391304347804</v>
+      </c>
+      <c r="K69">
+        <v>0.84412921475384495</v>
+      </c>
+      <c r="L69">
+        <v>0.686884875749464</v>
+      </c>
+      <c r="M69">
+        <v>0.86053550640279397</v>
+      </c>
+      <c r="N69">
+        <v>454.7</v>
+      </c>
+      <c r="O69">
+        <v>1023.7</v>
+      </c>
+      <c r="P69">
+        <v>126.3</v>
+      </c>
+      <c r="Q69">
+        <v>113.3</v>
+      </c>
+      <c r="R69">
+        <v>1150</v>
+      </c>
+      <c r="S69">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="70" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B70" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70" s="2">
+        <v>27</v>
+      </c>
+      <c r="D70" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70">
+        <v>3</v>
+      </c>
+      <c r="F70">
+        <v>4.5</v>
+      </c>
+      <c r="G70">
+        <v>0.93091036436007302</v>
+      </c>
+      <c r="H70">
+        <v>0.87782621270886396</v>
+      </c>
+      <c r="I70">
+        <v>0.81619718309859102</v>
+      </c>
+      <c r="J70">
+        <v>0.90756521739130402</v>
+      </c>
+      <c r="K70">
+        <v>0.86064776330940096</v>
+      </c>
+      <c r="L70">
+        <v>0.72321080654655401</v>
+      </c>
+      <c r="M70">
+        <v>0.877357392316647</v>
+      </c>
+      <c r="N70">
+        <v>463.6</v>
+      </c>
+      <c r="O70">
+        <v>1043.7</v>
+      </c>
+      <c r="P70">
+        <v>106.3</v>
+      </c>
+      <c r="Q70">
+        <v>104.4</v>
+      </c>
+      <c r="R70">
+        <v>1150</v>
+      </c>
+      <c r="S70">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="71" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B71" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="J42">
+      <c r="C71" s="2">
+        <v>6</v>
+      </c>
+      <c r="D71" t="s">
+        <v>16</v>
+      </c>
+      <c r="E71">
+        <v>32</v>
+      </c>
+      <c r="F71">
         <v>4.5</v>
       </c>
-      <c r="K42">
-        <v>0.87446037111000896</v>
-      </c>
-      <c r="L42">
-        <v>0.92001688433687701</v>
-      </c>
-      <c r="M42">
-        <v>0.81922739244951703</v>
-      </c>
-      <c r="N42">
-        <v>0.781174438687392</v>
-      </c>
-      <c r="O42">
-        <v>0.799890146966171</v>
-      </c>
-      <c r="P42">
-        <v>0.80640279394644898</v>
-      </c>
-      <c r="Q42">
-        <v>933.1</v>
-      </c>
-      <c r="R42">
-        <v>452.3</v>
-      </c>
-      <c r="S42">
-        <v>126.7</v>
-      </c>
-      <c r="T42">
-        <v>205.9</v>
-      </c>
-      <c r="U42">
-        <v>579</v>
-      </c>
-      <c r="V42">
-        <v>1139</v>
-      </c>
+      <c r="G71">
+        <v>0.75725264785475299</v>
+      </c>
+      <c r="H71">
+        <v>0.63448080521543604</v>
+      </c>
+      <c r="I71">
+        <v>0.691730474732006</v>
+      </c>
+      <c r="J71">
+        <v>0.68468976631748601</v>
+      </c>
+      <c r="K71">
+        <v>0.68802001254131195</v>
+      </c>
+      <c r="M71">
+        <v>0.68711721224920796</v>
+      </c>
+      <c r="N71">
+        <v>451.7</v>
+      </c>
+      <c r="O71">
+        <v>849.7</v>
+      </c>
+      <c r="P71">
+        <v>391.3</v>
+      </c>
+      <c r="Q71">
+        <v>201.3</v>
+      </c>
+      <c r="R71">
+        <v>1241</v>
+      </c>
+      <c r="S71">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="72" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B72" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C72" s="2">
+        <v>7</v>
+      </c>
+      <c r="D72" s="2"/>
+      <c r="E72" s="2"/>
+      <c r="F72" s="2"/>
+      <c r="G72" s="5"/>
+      <c r="H72" s="5"/>
+      <c r="I72" s="5"/>
+      <c r="J72" s="5"/>
+      <c r="K72" s="5"/>
+      <c r="L72" s="5"/>
+      <c r="M72" s="5"/>
+      <c r="N72" s="12"/>
+      <c r="O72" s="12"/>
+      <c r="P72" s="12"/>
+      <c r="Q72" s="12"/>
+      <c r="R72" s="15"/>
+      <c r="S72" s="15"/>
+    </row>
+    <row r="73" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B73" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C73" s="2">
+        <v>21</v>
+      </c>
+      <c r="D73" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73">
+        <v>14</v>
+      </c>
+      <c r="F73">
+        <v>4.5</v>
+      </c>
+      <c r="G73">
+        <v>0.89315370483772105</v>
+      </c>
+      <c r="H73">
+        <v>0.82933994498198804</v>
+      </c>
+      <c r="I73">
+        <v>0.77764084507042197</v>
+      </c>
+      <c r="J73">
+        <v>0.85678260869565204</v>
+      </c>
+      <c r="K73">
+        <v>0.81620575030111697</v>
+      </c>
+      <c r="M73">
+        <v>0.83061699650756604</v>
+      </c>
+      <c r="N73">
+        <v>441.7</v>
+      </c>
+      <c r="O73">
+        <v>985.3</v>
+      </c>
+      <c r="P73">
+        <v>164.7</v>
+      </c>
+      <c r="Q73">
+        <v>126.3</v>
+      </c>
+      <c r="R73">
+        <v>1150</v>
+      </c>
+      <c r="S73">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="74" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B74" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C74" s="2">
+        <v>27</v>
+      </c>
+      <c r="D74" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74">
+        <v>14</v>
+      </c>
+      <c r="F74">
+        <v>4.5</v>
+      </c>
+      <c r="G74">
+        <v>0.89506812614819298</v>
+      </c>
+      <c r="H74">
+        <v>0.82992320908998396</v>
+      </c>
+      <c r="I74">
+        <v>0.784330985915492</v>
+      </c>
+      <c r="J74">
+        <v>0.86191304347826103</v>
+      </c>
+      <c r="K74">
+        <v>0.82217013699168595</v>
+      </c>
+      <c r="L74">
+        <v>0.83626309662398102</v>
+      </c>
+      <c r="M74">
+        <v>445.5</v>
+      </c>
+      <c r="N74">
+        <v>991.2</v>
+      </c>
+      <c r="O74">
+        <v>158.80000000000001</v>
+      </c>
+      <c r="P74">
+        <v>122.5</v>
+      </c>
+      <c r="Q74">
+        <v>1150</v>
+      </c>
+      <c r="R74">
+        <v>568</v>
+      </c>
+      <c r="S74" s="15"/>
+    </row>
+    <row r="75" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B75" s="7"/>
+      <c r="C75" s="2"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="2"/>
+      <c r="F75" s="2"/>
+      <c r="G75" s="2"/>
+      <c r="H75" s="2"/>
+      <c r="I75" s="2"/>
+      <c r="J75" s="2"/>
+      <c r="K75" s="2"/>
+      <c r="L75" s="2"/>
+      <c r="M75" s="2"/>
+      <c r="N75" s="2"/>
+      <c r="O75" s="2"/>
+      <c r="P75" s="2"/>
+      <c r="Q75" s="2"/>
+      <c r="R75" s="15"/>
+      <c r="S75" s="15"/>
+    </row>
+    <row r="76" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B76" s="7"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="2"/>
+      <c r="N76" s="2"/>
+      <c r="O76" s="2"/>
+      <c r="P76" s="2"/>
+      <c r="Q76" s="2"/>
+      <c r="R76" s="15"/>
+      <c r="S76" s="15"/>
+    </row>
+    <row r="77" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B77" s="7"/>
+      <c r="C77" s="2"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2"/>
+      <c r="H77" s="2"/>
+      <c r="I77" s="2"/>
+      <c r="J77" s="2"/>
+      <c r="K77" s="2"/>
+      <c r="L77" s="2"/>
+      <c r="M77" s="2"/>
+      <c r="N77" s="2"/>
+      <c r="O77" s="2"/>
+      <c r="P77" s="2"/>
+      <c r="Q77" s="2"/>
+      <c r="R77" s="15"/>
+      <c r="S77" s="15"/>
+    </row>
+    <row r="78" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B78" s="7"/>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="2"/>
+      <c r="G78" s="2"/>
+      <c r="H78" s="2"/>
+      <c r="I78" s="2"/>
+      <c r="J78" s="2"/>
+      <c r="K78" s="2"/>
+      <c r="L78" s="2"/>
+      <c r="M78" s="2"/>
+      <c r="N78" s="2"/>
+      <c r="O78" s="2"/>
+      <c r="P78" s="2"/>
+      <c r="Q78" s="2"/>
+      <c r="R78" s="15"/>
+      <c r="S78" s="15"/>
+    </row>
+    <row r="79" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B79" s="7"/>
+      <c r="C79" s="2"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="2"/>
+      <c r="F79" s="2"/>
+      <c r="G79" s="2"/>
+      <c r="H79" s="2"/>
+      <c r="I79" s="2"/>
+      <c r="J79" s="2"/>
+      <c r="K79" s="2"/>
+      <c r="L79" s="2"/>
+      <c r="M79" s="2"/>
+      <c r="N79" s="2"/>
+      <c r="O79" s="2"/>
+      <c r="P79" s="2"/>
+      <c r="Q79" s="2"/>
+      <c r="R79" s="15"/>
+      <c r="S79" s="15"/>
+    </row>
+    <row r="80" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B80" s="7"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+      <c r="M80" s="2"/>
+      <c r="N80" s="2"/>
+      <c r="O80" s="2"/>
+      <c r="P80" s="2"/>
+      <c r="Q80" s="2"/>
+      <c r="R80" s="15"/>
+      <c r="S80" s="15"/>
+    </row>
+    <row r="81" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B81" s="7"/>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="2"/>
+      <c r="F81" s="2"/>
+      <c r="G81" s="2"/>
+      <c r="H81" s="2"/>
+      <c r="I81" s="2"/>
+      <c r="J81" s="2"/>
+      <c r="K81" s="2"/>
+      <c r="L81" s="2"/>
+      <c r="M81" s="2"/>
+      <c r="N81" s="2"/>
+      <c r="O81" s="2"/>
+      <c r="P81" s="2"/>
+      <c r="Q81" s="2"/>
+      <c r="R81" s="15"/>
+      <c r="S81" s="15"/>
+    </row>
+    <row r="82" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B82" s="7"/>
+      <c r="C82" s="2"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="2"/>
+      <c r="F82" s="2"/>
+      <c r="G82" s="2"/>
+      <c r="H82" s="2"/>
+      <c r="I82" s="2"/>
+      <c r="J82" s="2"/>
+      <c r="K82" s="2"/>
+      <c r="L82" s="2"/>
+      <c r="M82" s="2"/>
+      <c r="N82" s="2"/>
+      <c r="O82" s="2"/>
+      <c r="P82" s="2"/>
+      <c r="Q82" s="2"/>
+      <c r="R82" s="15"/>
+      <c r="S82" s="15"/>
+    </row>
+    <row r="83" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B83" s="7"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="2"/>
+      <c r="F83" s="2"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
+      <c r="I83" s="2"/>
+      <c r="J83" s="2"/>
+      <c r="K83" s="2"/>
+      <c r="L83" s="2"/>
+      <c r="M83" s="2"/>
+      <c r="N83" s="2"/>
+      <c r="O83" s="2"/>
+      <c r="P83" s="2"/>
+      <c r="Q83" s="2"/>
+      <c r="R83" s="15"/>
+      <c r="S83" s="15"/>
+    </row>
+    <row r="84" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B84" s="7"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="2"/>
+      <c r="F84" s="2"/>
+      <c r="G84" s="2"/>
+      <c r="H84" s="2"/>
+      <c r="I84" s="2"/>
+      <c r="J84" s="2"/>
+      <c r="K84" s="2"/>
+      <c r="L84" s="2"/>
+      <c r="M84" s="2"/>
+      <c r="N84" s="2"/>
+      <c r="O84" s="2"/>
+      <c r="P84" s="2"/>
+      <c r="Q84" s="2"/>
+      <c r="R84" s="15"/>
+      <c r="S84" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA928FA0-3D7A-684E-840A-12A28268388D}">
+  <dimension ref="B2:H52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="23.33203125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="60" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="18"/>
+      <c r="C4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+    </row>
+    <row r="5" spans="2:8" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B17" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B21" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="17"/>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B22" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B23" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B25" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B26" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="17" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B27" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B28" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B29" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B30" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B31" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B32" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C32" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C34" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C35" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="F35" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C37" s="17"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B38" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B40" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B41" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="C41" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F41" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42" s="18"/>
+      <c r="C42" s="17"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B43" s="18"/>
+      <c r="C43" s="17"/>
+      <c r="F43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44" s="18"/>
+      <c r="C44" s="17"/>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B45" s="18"/>
+      <c r="C45" s="17"/>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B46" s="18"/>
+      <c r="C46" s="17"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B47" s="18"/>
+      <c r="C47" s="17"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B48" s="18"/>
+      <c r="C48" s="17"/>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B49" s="18"/>
+      <c r="C49" s="17"/>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B50" s="18"/>
+      <c r="C50" s="17"/>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B51" s="18"/>
+      <c r="C51" s="17"/>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B52" s="18"/>
+      <c r="C52" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>